<commit_message>
Working template, spreadsheet, etc.
</commit_message>
<xml_diff>
--- a/copy_sheet/events.xlsx
+++ b/copy_sheet/events.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>firstFieldLabel</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Jordan Rudner</t>
+  </si>
+  <si>
+    <t>imageLink</t>
+  </si>
+  <si>
+    <t>http://dev.dailytexanonline.com/sites/default/files/images/2015/01/a%20different%20name.jpg</t>
   </si>
 </sst>
 </file>
@@ -456,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,8 +513,11 @@
       <c r="N1" t="s">
         <v>18</v>
       </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -545,8 +554,11 @@
       <c r="N2">
         <v>24</v>
       </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -582,6 +594,9 @@
       </c>
       <c r="N3">
         <v>13</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working template with all of the info we need
</commit_message>
<xml_diff>
--- a/copy_sheet/events.xlsx
+++ b/copy_sheet/events.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="19980" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -18,8 +18,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Where will the photo credit go?
+	-Amanda Voeller</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>firstFieldLabel</t>
   </si>
@@ -54,6 +76,27 @@
     <t>day</t>
   </si>
   <si>
+    <t>followYear</t>
+  </si>
+  <si>
+    <t>followMonth</t>
+  </si>
+  <si>
+    <t>followDay</t>
+  </si>
+  <si>
+    <t>imageLink</t>
+  </si>
+  <si>
+    <t>headlineLink</t>
+  </si>
+  <si>
+    <t>Leasing Office Opens:</t>
+  </si>
+  <si>
+    <t>Pointe on Rio leasing office opens. The building, located on Rio Grande Street, is scheduled to open on Aug. 16, before the start of the fall 2014 semester. The complex was still under construction by the end of the summer.</t>
+  </si>
+  <si>
     <t>Announcement Date:</t>
   </si>
   <si>
@@ -63,61 +106,179 @@
     <t>DT Coverage By:</t>
   </si>
   <si>
-    <t>Barbarians invaded the forest, leaving devestation and heart break in their wake. Life in Zilker park will never be the same for its historic residents.</t>
-  </si>
-  <si>
-    <t>La LA LAAAAAAA I wrote her off for the tenth time today, and practice all of the things i would say</t>
-  </si>
-  <si>
-    <t>followYear</t>
-  </si>
-  <si>
-    <t>followMonth</t>
-  </si>
-  <si>
-    <t>followDay</t>
-  </si>
-  <si>
-    <t>Look at this: It's a different headline, and that's exciting</t>
-  </si>
-  <si>
-    <t>Some suggest that Miles went insane while coding this project: Too long staying up, they said. Miles has not yet responded to requests for comment</t>
+    <t>Eleanor Dearman</t>
+  </si>
+  <si>
+    <t>Unfinished apartment complex relocates students to Dobie</t>
+  </si>
+  <si>
+    <t>http://www.dailytexanonline.com/2014/08/27/unfinished-apartment-complex-relocates-students-to-dobie</t>
+  </si>
+  <si>
+    <t>Announcement Date:</t>
+  </si>
+  <si>
+    <t>DT Coverage By:</t>
+  </si>
+  <si>
+    <t>Eleanor Dearman</t>
+  </si>
+  <si>
+    <t>Pointe on Rio leaseholders say construction delays likely to continue</t>
+  </si>
+  <si>
+    <t>The Daily Texan reports on indications that construction delays are likely to continue, though Pointe on Rio managers decline to comment on the situation. Ten days later, management will officially delay move-in by another three months.</t>
+  </si>
+  <si>
+    <t>Announcement Date:</t>
+  </si>
+  <si>
+    <t>New Move-In Date:</t>
+  </si>
+  <si>
+    <t>DT Coverage By:</t>
+  </si>
+  <si>
+    <t>Eleanor Dearman</t>
+  </si>
+  <si>
+    <t>Pointe on Rio futher delays move-in to January</t>
+  </si>
+  <si>
+    <t>http://www.dailytexanonline.com/2014/09/26/pointe-on-rio-futher-delays-move-in-to-january</t>
+  </si>
+  <si>
+    <t>Announcement Date:</t>
+  </si>
+  <si>
+    <t>DT Coverage By:</t>
   </si>
   <si>
     <t>Samantha Ketterer</t>
   </si>
   <si>
-    <t>Jordan Rudner</t>
-  </si>
-  <si>
-    <t>imageLink</t>
-  </si>
-  <si>
-    <t>http://dev.dailytexanonline.com/sites/default/files/images/2015/01/a%20different%20name.jpg</t>
+    <t>Announcement Date:</t>
+  </si>
+  <si>
+    <t>New Move-In Date:</t>
+  </si>
+  <si>
+    <t>DT Coverage By:</t>
+  </si>
+  <si>
+    <t>Samantha Ketterer</t>
+  </si>
+  <si>
+    <t>Pointe on Rio apartment building postpones move-in day for third time</t>
+  </si>
+  <si>
+    <t>http://www.dailytexanonline.com/2015/01/09/pointe-on-rio-apartment-building-postpones-move-in-day-for-third-time</t>
+  </si>
+  <si>
+    <t>Announcement Date:</t>
+  </si>
+  <si>
+    <t>New Move-In Date:</t>
+  </si>
+  <si>
+    <t>DT Coverage By:</t>
+  </si>
+  <si>
+    <t>Samantha Ketterer</t>
+  </si>
+  <si>
+    <t>Delayed again: Pointe on Rio managers postpone move-in day for the fourth time</t>
+  </si>
+  <si>
+    <t>http://www.dailytexanonline.com/2015/01/14/delayed-again-pointe-on-rio-managers-change-move-in-day-for-the-fourth-time</t>
+  </si>
+  <si>
+    <t>http://www.dailytexan.com/</t>
+  </si>
+  <si>
+    <t>Pointe on Rio management sends an email on Sept. 19 notifying leaseholders that move-in is now delayed to Jan. 10. The email cites 'city inspections and unforeseen construction delays' as the cause for the delay. Pointe on Rio management gives leaseholders the option to continue living at Dobie Center or at their outside housing accommodations, or to cancel their lease before Oct. 21.</t>
+  </si>
+  <si>
+    <t>On Jan. 2, Pointe on Rio management extends its room reservations at Dobie to Jan. 17, according to an email that Pointe on Rio managers sent to leaseholders. In the email, management said although they are taking 'precautionary measures,' they are still optimistic about a Jan. 10 move-in.</t>
+  </si>
+  <si>
+    <t>Because of ongoing construction, Pointe on Rio delays its move-in date to Oct. 15, according to an email Asset Campus Housing sent to leaseholders on July 24. The email gave two options for alternative housing: live at the Dobie Center off-campus residence hall rent-free, or receive a rent abatement worth twice the amount of residents' daily rent and stay at outside housing. Pointe on Rio management also gives leaseholders the option of opting out of their lease for free, after Oct. 15.</t>
+  </si>
+  <si>
+    <t>Pointe on Rio pushes back the move-in date for residents again, to Jan. 17, according to an email sent Jan. 7. The email attributes 'longer than anticipated delays with the City's inspections' as the reason for the change.</t>
+  </si>
+  <si>
+    <t>In an email sent to leaseholders, managers say the building will open Jan. 24, four days after the start of the spring semester. This is the fourth delay. Managers say they are waiting to receive a certificate of occupancy because of an 'inability to get sidewalks/drives poured,' most likely because of inclement weather. Stays at Dobie continue another week, and the email says Pointe on Rio will pro-rate leaseholders' rents from Jan. 10 until the day of move-in.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -126,18 +287,135 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -461,146 +739,328 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="15" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N1" t="s">
+      <c r="I2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="J2" s="2">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2">
+        <v>13</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2014</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2014</v>
+      </c>
+      <c r="M3" s="2">
+        <v>10</v>
+      </c>
+      <c r="N3" s="2">
+        <v>15</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
+    <row r="4" spans="1:16" ht="15" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="J4" s="2">
+        <v>9</v>
+      </c>
+      <c r="K4" s="2">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="6">
+        <v>2014</v>
+      </c>
+      <c r="J5" s="6">
+        <v>9</v>
+      </c>
+      <c r="K5" s="6">
+        <v>19</v>
+      </c>
+      <c r="L5" s="6">
+        <v>2015</v>
+      </c>
+      <c r="M5" s="6">
+        <v>1</v>
+      </c>
+      <c r="N5" s="6">
+        <v>10</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="6">
+        <v>2015</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="6">
+        <v>2015</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <v>7</v>
+      </c>
+      <c r="L7" s="6">
+        <v>2015</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>17</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="6">
+        <v>2015</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
         <v>14</v>
       </c>
-      <c r="I2">
-        <v>2014</v>
-      </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2">
-        <v>12</v>
-      </c>
-      <c r="L2">
-        <v>2014</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2">
+      <c r="L8" s="6">
+        <v>2015</v>
+      </c>
+      <c r="M8" s="6">
+        <v>1</v>
+      </c>
+      <c r="N8" s="6">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3">
-        <v>2014</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>2014</v>
-      </c>
-      <c r="M3">
-        <v>11</v>
-      </c>
-      <c r="N3">
-        <v>13</v>
-      </c>
-      <c r="O3" t="s">
-        <v>24</v>
+      <c r="P8" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1"/>
+    <hyperlink ref="P5" r:id="rId2"/>
+    <hyperlink ref="P7" r:id="rId3"/>
+    <hyperlink ref="P8" r:id="rId4"/>
+    <hyperlink ref="P4" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Large template with color changes.
</commit_message>
<xml_diff>
--- a/copy_sheet/events.xlsx
+++ b/copy_sheet/events.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>firstFieldLabel</t>
   </si>
@@ -211,16 +211,7 @@
     <t>In an email sent to leaseholders, managers say the building will open Jan. 24, four days after the start of the spring semester. This is the fourth delay. Managers say they are waiting to receive a certificate of occupancy because of an 'inability to get sidewalks/drives poured,' most likely because of inclement weather. Stays at Dobie continue another week, and the email says Pointe on Rio will pro-rate leaseholders' rents from Jan. 10 until the day of move-in.</t>
   </si>
   <si>
-    <t>http://i.huffpost.com/gen/460393/thumbs/s-RED-large.jpg</t>
-  </si>
-  <si>
     <t>photoAttribution</t>
-  </si>
-  <si>
-    <t>Peter Parker</t>
-  </si>
-  <si>
-    <t>Graham Hamilton</t>
   </si>
   <si>
     <t>photoAttributionLink</t>
@@ -771,7 +762,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -829,10 +820,10 @@
         <v>15</v>
       </c>
       <c r="Q1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
@@ -858,16 +849,9 @@
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O2" s="1"/>
       <c r="P2" s="2"/>
-      <c r="Q2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -906,14 +890,9 @@
       <c r="N3" s="2">
         <v>15</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O3" s="1"/>
       <c r="P3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
@@ -945,14 +924,9 @@
       <c r="L4" s="1"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O4" s="1"/>
       <c r="P4" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
@@ -992,14 +966,9 @@
       <c r="N5" s="6">
         <v>10</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O5" s="1"/>
       <c r="P5" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1">
@@ -1025,12 +994,7 @@
       <c r="K6" s="6">
         <v>2</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>58</v>
-      </c>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -1069,14 +1033,9 @@
       <c r="N7" s="6">
         <v>17</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O7" s="1"/>
       <c r="P7" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
@@ -1116,14 +1075,9 @@
       <c r="N8" s="6">
         <v>24</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="O8" s="1"/>
       <c r="P8" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>